<commit_message>
modified:   BoardView.cpp 	modified:   BoardView.h 	modified:   Game.cpp 	modified:   Game.h 	modified:   Menu.cpp
</commit_message>
<xml_diff>
--- a/23CLCChecklist.xlsx
+++ b/23CLCChecklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\Project_Programming_Techniques\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8947ED2C-5D86-45F9-913B-F276DBB6EC3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0454E163-F3EE-4EB4-9D3B-BAE66AC32902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rubrics" sheetId="1" r:id="rId1"/>
@@ -930,7 +930,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A21" sqref="A21:D21"/>
     </sheetView>
   </sheetViews>
@@ -1301,8 +1301,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1386,7 +1386,7 @@
         <v>12</v>
       </c>
       <c r="F8" s="9">
-        <v>201200001</v>
+        <v>23127216</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
@@ -1397,16 +1397,16 @@
         <v>14</v>
       </c>
       <c r="C9" s="9">
-        <v>201200001</v>
+        <v>23127216</v>
       </c>
       <c r="D9" s="9">
-        <v>201200002</v>
+        <v>23127216</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>15</v>
       </c>
       <c r="F9" s="9">
-        <v>201200001</v>
+        <v>23127216</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
@@ -1415,16 +1415,16 @@
         <v>16</v>
       </c>
       <c r="C10" s="9">
-        <v>201200001</v>
+        <v>23127216</v>
       </c>
       <c r="D10" s="9">
-        <v>201200002</v>
+        <v>23127216</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>18</v>
       </c>
       <c r="F10" s="9">
-        <v>201200001</v>
+        <v>23127216</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
@@ -1433,16 +1433,16 @@
         <v>17</v>
       </c>
       <c r="C11" s="9">
-        <v>201200001</v>
+        <v>23127216</v>
       </c>
       <c r="D11" s="9">
-        <v>201200002</v>
+        <v>23127216</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>20</v>
       </c>
       <c r="F11" s="9">
-        <v>201200001</v>
+        <v>23127216</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
@@ -1451,16 +1451,16 @@
         <v>19</v>
       </c>
       <c r="C12" s="9">
-        <v>201200001</v>
+        <v>23127216</v>
       </c>
       <c r="D12" s="9">
-        <v>201200002</v>
+        <v>23127216</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>22</v>
       </c>
       <c r="F12" s="9">
-        <v>201200001</v>
+        <v>23127216</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
@@ -1469,16 +1469,16 @@
         <v>21</v>
       </c>
       <c r="C13" s="9">
-        <v>201200001</v>
+        <v>23127216</v>
       </c>
       <c r="D13" s="9">
-        <v>201200002</v>
+        <v>23127216</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>24</v>
       </c>
       <c r="F13" s="9">
-        <v>201200001</v>
+        <v>23127216</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
@@ -1487,10 +1487,10 @@
         <v>23</v>
       </c>
       <c r="C14" s="9">
-        <v>201200001</v>
+        <v>23127216</v>
       </c>
       <c r="D14" s="9">
-        <v>201200002</v>
+        <v>23127216</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="16.8" x14ac:dyDescent="0.3">
@@ -1509,10 +1509,10 @@
         <v>26</v>
       </c>
       <c r="C16" s="9">
-        <v>201200001</v>
+        <v>23127216</v>
       </c>
       <c r="D16" s="9">
-        <v>201200002</v>
+        <v>23127223</v>
       </c>
       <c r="E16" s="34" t="s">
         <v>27</v>
@@ -1534,7 +1534,7 @@
         <v>29</v>
       </c>
       <c r="F17" s="9">
-        <v>201200001</v>
+        <v>23127223</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
@@ -1543,16 +1543,16 @@
         <v>30</v>
       </c>
       <c r="C18" s="9">
-        <v>201200001</v>
+        <v>23127216</v>
       </c>
       <c r="D18" s="9">
-        <v>201200002</v>
+        <v>23127223</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>31</v>
       </c>
       <c r="F18" s="9">
-        <v>201200001</v>
+        <v>23127223</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
@@ -1561,16 +1561,16 @@
         <v>32</v>
       </c>
       <c r="C19" s="9">
-        <v>201200001</v>
+        <v>23127216</v>
       </c>
       <c r="D19" s="9">
-        <v>201200002</v>
+        <v>23127223</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>33</v>
       </c>
       <c r="F19" s="9">
-        <v>201200001</v>
+        <v>23127223</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
@@ -1579,16 +1579,16 @@
         <v>34</v>
       </c>
       <c r="C20" s="9">
-        <v>201200001</v>
+        <v>23127216</v>
       </c>
       <c r="D20" s="9">
-        <v>201200002</v>
+        <v>23127223</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>35</v>
       </c>
       <c r="F20" s="9">
-        <v>201200001</v>
+        <v>23127223</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
@@ -1597,16 +1597,16 @@
         <v>36</v>
       </c>
       <c r="C21" s="9">
-        <v>201200001</v>
+        <v>23127216</v>
       </c>
       <c r="D21" s="9">
-        <v>201200002</v>
+        <v>23127223</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>37</v>
       </c>
       <c r="F21" s="9">
-        <v>201200001</v>
+        <v>23127223</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
@@ -1624,7 +1624,7 @@
         <v>39</v>
       </c>
       <c r="F22" s="9">
-        <v>201200001</v>
+        <v>23127223</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
@@ -1656,7 +1656,7 @@
         <v>43</v>
       </c>
       <c r="F24" s="9">
-        <v>201200001</v>
+        <v>23127223</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
@@ -1692,7 +1692,7 @@
         <v>47</v>
       </c>
       <c r="F26" s="9">
-        <v>201200001</v>
+        <v>23127223</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
@@ -1704,7 +1704,7 @@
         <v>48</v>
       </c>
       <c r="F27" s="9">
-        <v>201200001</v>
+        <v>23127223</v>
       </c>
     </row>
   </sheetData>
@@ -1728,7 +1728,7 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1775,7 +1775,7 @@
       </c>
       <c r="D3" s="16">
         <f>SUMIF('For students'!$C$9:$D$14,'For graders'!B3,'For graders'!$C$9:$D$14)+SUMIF('For students'!$F$8:$F$13,'For graders'!B3,'For graders'!$F$8:$F$13)+SUMIF('For students'!$C$16:$D$22,'For graders'!B3,'For graders'!$C$16:$D$22)+SUMIF('For students'!$C$24:$D$26,'For graders'!B3,'For graders'!$C$24:$D$26)+SUMIF('For students'!$F$17:$F$27,'For graders'!B3,'For graders'!$F$17:$F$27)</f>
-        <v>0</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="20.399999999999999" x14ac:dyDescent="0.35">
@@ -1792,7 +1792,7 @@
       </c>
       <c r="D4" s="16">
         <f>SUMIF('For students'!$C$9:$D$14,'For graders'!B4,'For graders'!$C$9:$D$14)+SUMIF('For students'!$F$8:$F$13,'For graders'!B4,'For graders'!$F$8:$F$13)+SUMIF('For students'!$C$16:$D$22,'For graders'!B4,'For graders'!$C$16:$D$22)+SUMIF('For students'!$C$24:$D$26,'For graders'!B4,'For graders'!$C$24:$D$26)+SUMIF('For students'!$F$17:$F$27,'For graders'!B4,'For graders'!$F$17:$F$27)</f>
-        <v>0</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="18" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Add more comment 	modified:   .vscode/c_cpp_properties.json 	modified:   .vscode/launch.json 	modified:   .vscode/tasks.json 	modified:   23CLCChecklist.xlsx 	modified:   BoardView.cpp 	modified:   Controller.cpp 	modified:   Game.cpp 	modified:   Menu.cpp 	modified:   out.exe 	modified:   rank/leaderboard.txt
</commit_message>
<xml_diff>
--- a/23CLCChecklist.xlsx
+++ b/23CLCChecklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\Project_Programming_Techniques\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0454E163-F3EE-4EB4-9D3B-BAE66AC32902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2768DB79-142F-4F2B-B37A-34B2421784EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rubrics" sheetId="1" r:id="rId1"/>
@@ -1301,8 +1301,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1525,10 +1525,10 @@
         <v>28</v>
       </c>
       <c r="C17" s="9">
-        <v>201200001</v>
+        <v>23127216</v>
       </c>
       <c r="D17" s="9">
-        <v>201200002</v>
+        <v>23127223</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>29</v>
@@ -1727,7 +1727,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
@@ -1775,7 +1775,7 @@
       </c>
       <c r="D3" s="16">
         <f>SUMIF('For students'!$C$9:$D$14,'For graders'!B3,'For graders'!$C$9:$D$14)+SUMIF('For students'!$F$8:$F$13,'For graders'!B3,'For graders'!$F$8:$F$13)+SUMIF('For students'!$C$16:$D$22,'For graders'!B3,'For graders'!$C$16:$D$22)+SUMIF('For students'!$C$24:$D$26,'For graders'!B3,'For graders'!$C$24:$D$26)+SUMIF('For students'!$F$17:$F$27,'For graders'!B3,'For graders'!$F$17:$F$27)</f>
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="20.399999999999999" x14ac:dyDescent="0.35">
@@ -1792,7 +1792,7 @@
       </c>
       <c r="D4" s="16">
         <f>SUMIF('For students'!$C$9:$D$14,'For graders'!B4,'For graders'!$C$9:$D$14)+SUMIF('For students'!$F$8:$F$13,'For graders'!B4,'For graders'!$F$8:$F$13)+SUMIF('For students'!$C$16:$D$22,'For graders'!B4,'For graders'!$C$16:$D$22)+SUMIF('For students'!$C$24:$D$26,'For graders'!B4,'For graders'!$C$24:$D$26)+SUMIF('For students'!$F$17:$F$27,'For graders'!B4,'For graders'!$F$17:$F$27)</f>
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="18" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Finish project 	modified:   .vscode/settings.json 	modified:   23CLCChecklist.xlsx 	modified:   BoardView.cpp 	modified:   BoardView.h 	modified:   Controller.cpp 	modified:   Controller.h 	modified:   Game.cpp 	modified:   Game.h 	modified:   Menu.cpp 	modified:   Menu.h 	modified:   Point.cpp 	modified:   Point.h 	new file:   leaderboard.txt 	deleted:    lose.wav 	modified:   out.exe 	modified:   rank/leaderboard.txt 	renamed:    background.wav -> sound/background.wav 	renamed:    effect.wav -> sound/effect.wav 	renamed:    enter.wav -> sound/enter.wav 	renamed:    error.wav -> sound/error.wav 	new file:   sound/lose.wav 	renamed:    move.wav -> sound/move.wav 	renamed:    placed.wav -> sound/placed.wav 	renamed:    win.wav -> sound/win.wav
</commit_message>
<xml_diff>
--- a/23CLCChecklist.xlsx
+++ b/23CLCChecklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\Project_Programming_Techniques\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2768DB79-142F-4F2B-B37A-34B2421784EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C27806-F956-4468-B8D2-5AF974A328A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rubrics" sheetId="1" r:id="rId1"/>
@@ -1301,8 +1301,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1647,10 +1647,10 @@
         <v>42</v>
       </c>
       <c r="C24" s="9">
-        <v>201200001</v>
+        <v>23127216</v>
       </c>
       <c r="D24" s="9">
-        <v>201200001</v>
+        <v>23127223</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>43</v>
@@ -1665,16 +1665,16 @@
         <v>44</v>
       </c>
       <c r="C25" s="9">
-        <v>201200001</v>
+        <v>23127216</v>
       </c>
       <c r="D25" s="9">
-        <v>201200001</v>
+        <v>23127223</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>45</v>
       </c>
       <c r="F25" s="9">
-        <v>201200001</v>
+        <v>23127223</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
@@ -1683,10 +1683,10 @@
         <v>46</v>
       </c>
       <c r="C26" s="9">
-        <v>201200001</v>
+        <v>23127216</v>
       </c>
       <c r="D26" s="9">
-        <v>201200001</v>
+        <v>23217223</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>47</v>
@@ -1727,7 +1727,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
@@ -1792,7 +1792,7 @@
       </c>
       <c r="D4" s="16">
         <f>SUMIF('For students'!$C$9:$D$14,'For graders'!B4,'For graders'!$C$9:$D$14)+SUMIF('For students'!$F$8:$F$13,'For graders'!B4,'For graders'!$F$8:$F$13)+SUMIF('For students'!$C$16:$D$22,'For graders'!B4,'For graders'!$C$16:$D$22)+SUMIF('For students'!$C$24:$D$26,'For graders'!B4,'For graders'!$C$24:$D$26)+SUMIF('For students'!$F$17:$F$27,'For graders'!B4,'For graders'!$F$17:$F$27)</f>
-        <v>80</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="18" x14ac:dyDescent="0.35">

</xml_diff>